<commit_message>
finalmente lungo il giusto
</commit_message>
<xml_diff>
--- a/STDCXX-TicketFixed.xlsx
+++ b/STDCXX-TicketFixed.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Costa\eclipse-workspace\ISW2_Deliverable1_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E656EC2C-FD4F-4D7B-B63C-49BF3E2A1317}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C4254-9EB6-4ED2-B17F-A2160A77DD7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STDCXX-TicketFixed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -610,7 +621,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -991,7 +1002,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E429-41FB-B82E-BAECFDF6127A}"/>
+              <c16:uniqueId val="{00000000-C089-4FF8-A8F1-B662633C554D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1193,160 +1204,160 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>11.65384615</c:v>
+                  <c:v>11.653846153846153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,7 +1365,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E429-41FB-B82E-BAECFDF6127A}"/>
+              <c16:uniqueId val="{00000001-C089-4FF8-A8F1-B662633C554D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1556,7 +1567,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>12.845819669999999</c:v>
+                  <c:v>12.845819668524832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1564,7 +1575,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E429-41FB-B82E-BAECFDF6127A}"/>
+              <c16:uniqueId val="{00000002-C089-4FF8-A8F1-B662633C554D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1766,160 +1777,160 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>50.191305159999999</c:v>
+                  <c:v>50.191305159420651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,7 +1938,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E429-41FB-B82E-BAECFDF6127A}"/>
+              <c16:uniqueId val="{00000003-C089-4FF8-A8F1-B662633C554D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2290,7 +2301,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-E429-41FB-B82E-BAECFDF6127A}"/>
+              <c16:uniqueId val="{00000004-C089-4FF8-A8F1-B662633C554D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2302,11 +2313,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1277184496"/>
-        <c:axId val="1277169936"/>
+        <c:axId val="912785440"/>
+        <c:axId val="912782112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1277184496"/>
+        <c:axId val="912785440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2348,7 +2359,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="sng" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2363,12 +2374,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277169936"/>
+        <c:crossAx val="912782112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1277169936"/>
+        <c:axId val="912782112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,7 +2421,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="sng" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2425,7 +2436,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277184496"/>
+        <c:crossAx val="912785440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2452,7 +2463,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" u="sng" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2499,7 +2510,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr u="sng"/>
       </a:pPr>
       <a:endParaRPr lang="it-IT"/>
     </a:p>
@@ -3072,23 +3083,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
+        <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B900895-A595-4FFB-84C5-B4E866954BF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{463AB8A4-39F5-4DC0-901C-3CAD45CE34CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3405,11 +3416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,15 +3456,19 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>11.65384615</v>
+        <f>AVERAGE($B$2:$B$53)</f>
+        <v>11.653846153846153</v>
       </c>
       <c r="D2">
-        <v>12.845819669999999</v>
+        <f>_xlfn.STDEV.S($B$2:$B$53)</f>
+        <v>12.845819668524832</v>
       </c>
       <c r="E2">
-        <v>50.191305159999999</v>
+        <f>$C$2+$D$2*3</f>
+        <v>50.191305159420651</v>
       </c>
       <c r="F2">
+        <f>IF($C$2-$D$2*3&lt;0,0,$C$2-$D$2*3)</f>
         <v>0</v>
       </c>
     </row>
@@ -3465,12 +3480,15 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>11.65384615</v>
+        <f t="shared" ref="C3:C53" si="0">AVERAGE($B$2:$B$53)</f>
+        <v>11.653846153846153</v>
       </c>
       <c r="E3">
-        <v>50.191305159999999</v>
+        <f t="shared" ref="E3:E53" si="1">$C$2+$D$2*3</f>
+        <v>50.191305159420651</v>
       </c>
       <c r="F3">
+        <f t="shared" ref="F3:F53" si="2">IF($C$2-$D$2*3&lt;0,0,$C$2-$D$2*3)</f>
         <v>0</v>
       </c>
     </row>
@@ -3482,12 +3500,15 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E4">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F4">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3499,12 +3520,15 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E5">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3516,12 +3540,15 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E6">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3533,12 +3560,15 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E7">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F7">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3550,12 +3580,15 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E8">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3567,12 +3600,15 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E9">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3584,12 +3620,15 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E10">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3601,12 +3640,15 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E11">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F11">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3618,12 +3660,15 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E12">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F12">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3635,12 +3680,15 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E13">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F13">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3652,12 +3700,15 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E14">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3669,12 +3720,15 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E15">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F15">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3686,12 +3740,15 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E16">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F16">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3703,12 +3760,15 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E17">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F17">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3720,12 +3780,15 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E18">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F18">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3737,12 +3800,15 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E19">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F19">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3754,12 +3820,15 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E20">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F20">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3771,12 +3840,15 @@
         <v>28</v>
       </c>
       <c r="C21">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E21">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F21">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3788,12 +3860,15 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E22">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F22">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3805,12 +3880,15 @@
         <v>18</v>
       </c>
       <c r="C23">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E23">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F23">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3822,12 +3900,15 @@
         <v>18</v>
       </c>
       <c r="C24">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E24">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F24">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3839,12 +3920,15 @@
         <v>12</v>
       </c>
       <c r="C25">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E25">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F25">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3856,12 +3940,15 @@
         <v>34</v>
       </c>
       <c r="C26">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E26">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F26">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3873,12 +3960,15 @@
         <v>40</v>
       </c>
       <c r="C27">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E27">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F27">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3890,12 +3980,15 @@
         <v>35</v>
       </c>
       <c r="C28">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E28">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F28">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3907,12 +4000,15 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E29">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F29">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3924,12 +4020,15 @@
         <v>15</v>
       </c>
       <c r="C30">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E30">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F30">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3941,12 +4040,15 @@
         <v>11</v>
       </c>
       <c r="C31">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E31">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F31">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3958,12 +4060,15 @@
         <v>22</v>
       </c>
       <c r="C32">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E32">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F32">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3975,12 +4080,15 @@
         <v>42</v>
       </c>
       <c r="C33">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E33">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F33">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3992,12 +4100,15 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E34">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F34">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4009,12 +4120,15 @@
         <v>27</v>
       </c>
       <c r="C35">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E35">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F35">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4026,12 +4140,15 @@
         <v>13</v>
       </c>
       <c r="C36">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E36">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F36">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4043,12 +4160,15 @@
         <v>25</v>
       </c>
       <c r="C37">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E37">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F37">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4060,12 +4180,15 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E38">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F38">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4077,12 +4200,15 @@
         <v>7</v>
       </c>
       <c r="C39">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E39">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F39">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4094,12 +4220,15 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E40">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F40">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4111,12 +4240,15 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E41">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4128,12 +4260,15 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E42">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F42">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4145,12 +4280,15 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E43">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F43">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4162,12 +4300,15 @@
         <v>2</v>
       </c>
       <c r="C44">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E44">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F44">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4179,12 +4320,15 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E45">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F45">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4196,12 +4340,15 @@
         <v>2</v>
       </c>
       <c r="C46">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E46">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F46">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4213,12 +4360,15 @@
         <v>2</v>
       </c>
       <c r="C47">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E47">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F47">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4230,12 +4380,15 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E48">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F48">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4247,12 +4400,15 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E49">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F49">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4264,12 +4420,15 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E50">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4281,12 +4440,15 @@
         <v>2</v>
       </c>
       <c r="C51">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E51">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F51">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4298,12 +4460,15 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E52">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F52">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4315,12 +4480,15 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>11.65384615</v>
+        <f t="shared" si="0"/>
+        <v>11.653846153846153</v>
       </c>
       <c r="E53">
-        <v>50.191305159999999</v>
+        <f t="shared" si="1"/>
+        <v>50.191305159420651</v>
       </c>
       <c r="F53">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>